<commit_message>
Validation changes added  for empty and details error summary
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_4.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet state="visible" name="API-Testing" sheetId="1" r:id="rId4"/>
@@ -256,6 +256,30 @@
   </si>
   <si>
     <t>Tags</t>
+  </si>
+  <si>
+    <t>PetEmptyTest</t>
+  </si>
+  <si>
+    <t>API get testing</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/api/pets/findByTags?tags=light-grey</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>get_response_empty.json</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>PetGetTest</t>
+  </si>
+  <si>
+    <t>Testing Empty</t>
   </si>
 </sst>
 </file>
@@ -577,7 +601,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="topLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -733,6 +757,29 @@
         <v>33</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="0">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -744,6 +791,7 @@
     <hyperlink ref="M2" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
     <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
@@ -756,7 +804,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="topLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -917,6 +965,29 @@
         <v>33</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="0">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G3">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -928,6 +999,7 @@
     <hyperlink ref="M2" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
     <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>

</xml_diff>